<commit_message>
update tr tc br
</commit_message>
<xml_diff>
--- a/template-dung/OJT_Template_Group5_User-1234.xlsx
+++ b/template-dung/OJT_Template_Group5_User-1234.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" tabRatio="355" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" tabRatio="355" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TR List" sheetId="2" r:id="rId1"/>
@@ -1916,33 +1916,16 @@
     <t>"Tìm kiếm sản phẩm"</t>
   </si>
   <si>
-    <t>1. Navigate to Điện máy đỏ web.
-2. On textbox "Nhập tên sản phẩm cần tìm", input: "acer", click on "Tìm".
-3. Observe the program's result.
-Observed Result: "không có dữ liệu".
-Expected Result: the products name with "acer"</t>
-  </si>
-  <si>
     <t>Bug-0003</t>
   </si>
   <si>
     <t>User can not use the Enter key for searching like "Tìm" button.</t>
   </si>
   <si>
-    <t>1. Navigate to Điện máy đỏ web.
-2. On textbox "Nhập tên sản phẩm cần tìm", input: "acer", press Enter key.
-3. Observe the program's result.
-Observed Result: the homepage is loaded.
-Expected Result: the products name with "acer"</t>
-  </si>
-  <si>
     <t>Bug-0004</t>
   </si>
   <si>
     <t>The linking from product's image to the product detail page is not avaiable.</t>
-  </si>
-  <si>
-    <t>User can not view the product detail page by click on the product's image.</t>
   </si>
   <si>
     <t>Home, Sản phẩm</t>
@@ -1964,21 +1947,10 @@
     <t>Home, Yêu thích</t>
   </si>
   <si>
-    <t>1. Navigate to Điện máy đỏ web, "section "Bán nhiều nhất".
-2. Click on "yêu thích" button of "Canon 750D + Lens 18-55".
-3. Click on "Yêu thích" button.
-4. Observe the list "Yêu thích".
-Observed Result: the selected item is not add to "Yêu thích". 
-Expected Result: "Thêm vào giỏ hàng thành công" message is displayed.</t>
-  </si>
-  <si>
     <t>Bug-0006</t>
   </si>
   <si>
     <t>The mobile phone number does not follow the format "+84 xxx xxxxxx".</t>
-  </si>
-  <si>
-    <t>The mobile phone number does not follows the format "+84 xxx xxxxxx".</t>
   </si>
   <si>
     <t>1. Navigate to Điện máy đỏ web, 
@@ -2039,9 +2011,6 @@
     <t>Bug-0010</t>
   </si>
   <si>
-    <t>Account is valid when user do not active account.</t>
-  </si>
-  <si>
     <t>1. Navigate to Điện máy đỏ web.
 2. Click on "Đăng ký" link.
 3. Input information: group05dung8/123456, Dương Tuấn Dũng, dtdung8@gmail.com, An Giang, 12345678, Nam, 11/11/1983
@@ -2070,27 +2039,10 @@
     <t>Bug-0011</t>
   </si>
   <si>
-    <t xml:space="preserve">The textbox's length is used more space in the form. . </t>
-  </si>
-  <si>
-    <t>1. Navigate to Điện máy đỏ web, 
-2. Click on "Đăng nhập" link.
-3. Observe the form "Đăng nhập".
-Observed Result: the length of textbox in the form almost equal the width of the page.
-Expected Result: the length of textbox in the form fixed nicely the width of the page.</t>
-  </si>
-  <si>
     <t>Bug-0012</t>
   </si>
   <si>
     <t>User can not select the year before 1970.</t>
-  </si>
-  <si>
-    <t>1. Navigate to Điện máy đỏ web.
-2. Click on "Đăng ký".
-3. Observe the "chọn năm" listbox.
-Observed Result: a fixed year form 1970 to 2018.
-Expected Result: Datetime picker.</t>
   </si>
   <si>
     <t>Bug-0013</t>
@@ -2154,6 +2106,54 @@
 5. Observe account information.
 Observed Result: "Cập nhật thành công" message is displayed.
 Expected Result: Error message is displayed.</t>
+  </si>
+  <si>
+    <t>1. Navigate to Điện máy đỏ web.
+2. On textbox "Nhập tên sản phẩm cần tìm", input: "acer", click on "Tìm".
+3. Observe the program's result.
+Observed Result: "không có dữ liệu".
+Expected Result: the products name with "acer" is displayed.</t>
+  </si>
+  <si>
+    <t>1. Navigate to Điện máy đỏ web.
+2. On textbox "Nhập tên sản phẩm cần tìm", input: "acer", press Enter key.
+3. Observe the program's result.
+Observed Result: the homepage is loaded.
+Expected Result: the products name with "acer" is displayed</t>
+  </si>
+  <si>
+    <t>User can not view the product detail by click on the product's image.</t>
+  </si>
+  <si>
+    <t>1. Navigate to Điện máy đỏ web, "section "Bán nhiều nhất".
+2. Click on "yêu thích" button of "Canon 750D + Lens 18-55".
+3. Click on "Yêu thích" button.
+4. Observe the list "Yêu thích".
+Observed Result: the page is reloaded.
+Expected Result: "Thêm vào giỏ hàng thành công" message is displayed.</t>
+  </si>
+  <si>
+    <t>An account is always valid when user do not active account.</t>
+  </si>
+  <si>
+    <t>Account is always valid when user do not active account.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The textbox's length use more space in the form. . </t>
+  </si>
+  <si>
+    <t>1. Navigate to Điện máy đỏ web, 
+2. Click on "Đăng nhập" link.
+3. Observe the form "Đăng nhập".
+Observed Result: the length of textbox almost equal the width of the page.
+Expected Result: the length of textbox fixed nicely the width of the page.</t>
+  </si>
+  <si>
+    <t>1. Navigate to Điện máy đỏ web.
+2. Click on "Đăng ký".
+3. Observe the "chọn năm" listbox.
+Observed Result: a fixed year form 1970 to 2018.
+Expected Result: use Datetime picker for "Ngày sinh" info.</t>
   </si>
 </sst>
 </file>
@@ -2464,11 +2464,11 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -2957,10 +2957,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="46"/>
+      <c r="B1" s="47"/>
     </row>
     <row r="4" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
@@ -4118,7 +4118,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K94"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
       <selection activeCell="F42" sqref="F42"/>
     </sheetView>
   </sheetViews>
@@ -6509,8 +6509,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView showGridLines="0" topLeftCell="A21" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6610,7 +6610,7 @@
       <c r="B7" s="34" t="s">
         <v>483</v>
       </c>
-      <c r="C7" s="47" t="s">
+      <c r="C7" s="46" t="s">
         <v>490</v>
       </c>
       <c r="D7" s="32" t="s">
@@ -6626,22 +6626,22 @@
         <v>488</v>
       </c>
       <c r="H7" s="33" t="s">
-        <v>494</v>
+        <v>538</v>
       </c>
       <c r="I7" s="24"/>
     </row>
     <row r="8" spans="1:9" ht="121.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="26" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B8" s="34" t="s">
         <v>483</v>
       </c>
-      <c r="C8" s="47" t="s">
-        <v>496</v>
-      </c>
-      <c r="D8" s="47" t="s">
-        <v>496</v>
+      <c r="C8" s="46" t="s">
+        <v>495</v>
+      </c>
+      <c r="D8" s="46" t="s">
+        <v>495</v>
       </c>
       <c r="E8" s="32" t="s">
         <v>492</v>
@@ -6653,75 +6653,75 @@
         <v>488</v>
       </c>
       <c r="H8" s="33" t="s">
-        <v>497</v>
+        <v>539</v>
       </c>
       <c r="I8" s="24"/>
     </row>
     <row r="9" spans="1:9" ht="120" x14ac:dyDescent="0.2">
       <c r="A9" s="26" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="B9" s="34" t="s">
         <v>483</v>
       </c>
-      <c r="C9" s="47" t="s">
-        <v>499</v>
-      </c>
-      <c r="D9" s="47" t="s">
-        <v>500</v>
+      <c r="C9" s="46" t="s">
+        <v>497</v>
+      </c>
+      <c r="D9" s="46" t="s">
+        <v>540</v>
       </c>
       <c r="E9" s="32" t="s">
         <v>486</v>
       </c>
       <c r="F9" s="32" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="G9" s="32" t="s">
         <v>488</v>
       </c>
       <c r="H9" s="33" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="I9" s="24"/>
     </row>
-    <row r="10" spans="1:9" ht="165" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" ht="150" x14ac:dyDescent="0.2">
       <c r="A10" s="26" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="B10" s="34" t="s">
         <v>483</v>
       </c>
-      <c r="C10" s="47" t="s">
-        <v>504</v>
-      </c>
-      <c r="D10" s="47" t="s">
-        <v>504</v>
+      <c r="C10" s="46" t="s">
+        <v>501</v>
+      </c>
+      <c r="D10" s="46" t="s">
+        <v>501</v>
       </c>
       <c r="E10" s="32" t="s">
         <v>492</v>
       </c>
       <c r="F10" s="32" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="G10" s="32" t="s">
         <v>488</v>
       </c>
       <c r="H10" s="33" t="s">
-        <v>506</v>
+        <v>541</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="75" x14ac:dyDescent="0.2">
       <c r="A11" s="26" t="s">
-        <v>507</v>
+        <v>503</v>
       </c>
       <c r="B11" s="34" t="s">
         <v>483</v>
       </c>
-      <c r="C11" s="47" t="s">
-        <v>508</v>
-      </c>
-      <c r="D11" s="47" t="s">
-        <v>509</v>
+      <c r="C11" s="46" t="s">
+        <v>504</v>
+      </c>
+      <c r="D11" s="46" t="s">
+        <v>504</v>
       </c>
       <c r="E11" s="32" t="s">
         <v>486</v>
@@ -6733,21 +6733,21 @@
         <v>488</v>
       </c>
       <c r="H11" s="33" t="s">
-        <v>510</v>
+        <v>505</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="90" x14ac:dyDescent="0.2">
       <c r="A12" s="26" t="s">
-        <v>511</v>
+        <v>506</v>
       </c>
       <c r="B12" s="34" t="s">
         <v>483</v>
       </c>
-      <c r="C12" s="47" t="s">
-        <v>512</v>
-      </c>
-      <c r="D12" s="47" t="s">
-        <v>512</v>
+      <c r="C12" s="46" t="s">
+        <v>507</v>
+      </c>
+      <c r="D12" s="46" t="s">
+        <v>507</v>
       </c>
       <c r="E12" s="32" t="s">
         <v>486</v>
@@ -6759,271 +6759,271 @@
         <v>488</v>
       </c>
       <c r="H12" s="33" t="s">
-        <v>513</v>
+        <v>508</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="75" x14ac:dyDescent="0.2">
       <c r="A13" s="26" t="s">
-        <v>514</v>
+        <v>509</v>
       </c>
       <c r="B13" s="34" t="s">
         <v>483</v>
       </c>
-      <c r="C13" s="47" t="s">
-        <v>515</v>
-      </c>
-      <c r="D13" s="47" t="s">
-        <v>515</v>
+      <c r="C13" s="46" t="s">
+        <v>510</v>
+      </c>
+      <c r="D13" s="46" t="s">
+        <v>510</v>
       </c>
       <c r="E13" s="32" t="s">
         <v>486</v>
       </c>
       <c r="F13" s="32" t="s">
-        <v>516</v>
+        <v>511</v>
       </c>
       <c r="G13" s="32" t="s">
         <v>488</v>
       </c>
       <c r="H13" s="33" t="s">
-        <v>517</v>
+        <v>512</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="195" x14ac:dyDescent="0.2">
       <c r="A14" s="26" t="s">
-        <v>518</v>
+        <v>513</v>
       </c>
       <c r="B14" s="34" t="s">
         <v>483</v>
       </c>
-      <c r="C14" s="47" t="s">
-        <v>519</v>
-      </c>
-      <c r="D14" s="47" t="s">
-        <v>519</v>
+      <c r="C14" s="46" t="s">
+        <v>514</v>
+      </c>
+      <c r="D14" s="46" t="s">
+        <v>514</v>
       </c>
       <c r="E14" s="32" t="s">
         <v>492</v>
       </c>
       <c r="F14" s="32" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
       <c r="G14" s="32" t="s">
         <v>488</v>
       </c>
       <c r="H14" s="33" t="s">
-        <v>521</v>
+        <v>516</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="225" x14ac:dyDescent="0.2">
       <c r="A15" s="26" t="s">
-        <v>522</v>
+        <v>517</v>
       </c>
       <c r="B15" s="34" t="s">
         <v>483</v>
       </c>
-      <c r="C15" s="47" t="s">
-        <v>523</v>
-      </c>
-      <c r="D15" s="47" t="s">
-        <v>523</v>
+      <c r="C15" s="46" t="s">
+        <v>542</v>
+      </c>
+      <c r="D15" s="46" t="s">
+        <v>543</v>
       </c>
       <c r="E15" s="32" t="s">
         <v>492</v>
       </c>
       <c r="F15" s="32" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
       <c r="G15" s="32" t="s">
         <v>488</v>
       </c>
       <c r="H15" s="33" t="s">
-        <v>524</v>
+        <v>518</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="180" x14ac:dyDescent="0.2">
       <c r="A16" s="26" t="s">
-        <v>522</v>
+        <v>517</v>
       </c>
       <c r="B16" s="34" t="s">
         <v>483</v>
       </c>
-      <c r="C16" s="47" t="s">
-        <v>525</v>
-      </c>
-      <c r="D16" s="47" t="s">
-        <v>525</v>
+      <c r="C16" s="46" t="s">
+        <v>519</v>
+      </c>
+      <c r="D16" s="46" t="s">
+        <v>519</v>
       </c>
       <c r="E16" s="32" t="s">
         <v>486</v>
       </c>
       <c r="F16" s="32" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
       <c r="G16" s="32" t="s">
         <v>488</v>
       </c>
       <c r="H16" s="33" t="s">
-        <v>526</v>
+        <v>520</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="120" x14ac:dyDescent="0.2">
       <c r="A17" s="26" t="s">
-        <v>527</v>
+        <v>521</v>
       </c>
       <c r="B17" s="34" t="s">
         <v>483</v>
       </c>
-      <c r="C17" s="47" t="s">
-        <v>528</v>
-      </c>
-      <c r="D17" s="47" t="s">
-        <v>528</v>
+      <c r="C17" s="46" t="s">
+        <v>544</v>
+      </c>
+      <c r="D17" s="46" t="s">
+        <v>544</v>
       </c>
       <c r="E17" s="32" t="s">
         <v>486</v>
       </c>
       <c r="F17" s="32" t="s">
-        <v>516</v>
+        <v>511</v>
       </c>
       <c r="G17" s="32" t="s">
         <v>488</v>
       </c>
       <c r="H17" s="33" t="s">
-        <v>529</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="105" x14ac:dyDescent="0.2">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="120" x14ac:dyDescent="0.2">
       <c r="A18" s="26" t="s">
-        <v>530</v>
+        <v>522</v>
       </c>
       <c r="B18" s="34" t="s">
         <v>483</v>
       </c>
-      <c r="C18" s="47" t="s">
-        <v>531</v>
-      </c>
-      <c r="D18" s="47" t="s">
-        <v>531</v>
+      <c r="C18" s="46" t="s">
+        <v>523</v>
+      </c>
+      <c r="D18" s="46" t="s">
+        <v>523</v>
       </c>
       <c r="E18" s="32" t="s">
         <v>486</v>
       </c>
       <c r="F18" s="32" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
       <c r="G18" s="32" t="s">
         <v>488</v>
       </c>
       <c r="H18" s="33" t="s">
-        <v>532</v>
+        <v>546</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="135" x14ac:dyDescent="0.2">
       <c r="A19" s="26" t="s">
-        <v>533</v>
+        <v>524</v>
       </c>
       <c r="B19" s="34" t="s">
         <v>483</v>
       </c>
-      <c r="C19" s="47" t="s">
-        <v>534</v>
-      </c>
-      <c r="D19" s="47" t="s">
-        <v>534</v>
+      <c r="C19" s="46" t="s">
+        <v>525</v>
+      </c>
+      <c r="D19" s="46" t="s">
+        <v>525</v>
       </c>
       <c r="E19" s="32" t="s">
         <v>486</v>
       </c>
       <c r="F19" s="32" t="s">
-        <v>535</v>
+        <v>526</v>
       </c>
       <c r="G19" s="32" t="s">
         <v>488</v>
       </c>
       <c r="H19" s="33" t="s">
-        <v>536</v>
+        <v>527</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="120" x14ac:dyDescent="0.2">
       <c r="A20" s="26" t="s">
-        <v>537</v>
+        <v>528</v>
       </c>
       <c r="B20" s="34" t="s">
         <v>483</v>
       </c>
-      <c r="C20" s="47" t="s">
-        <v>538</v>
-      </c>
-      <c r="D20" s="47" t="s">
-        <v>538</v>
+      <c r="C20" s="46" t="s">
+        <v>529</v>
+      </c>
+      <c r="D20" s="46" t="s">
+        <v>529</v>
       </c>
       <c r="E20" s="32" t="s">
         <v>486</v>
       </c>
       <c r="F20" s="32" t="s">
-        <v>535</v>
+        <v>526</v>
       </c>
       <c r="G20" s="32" t="s">
         <v>488</v>
       </c>
       <c r="H20" s="33" t="s">
-        <v>539</v>
+        <v>530</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="150" x14ac:dyDescent="0.2">
       <c r="A21" s="26" t="s">
-        <v>540</v>
+        <v>531</v>
       </c>
       <c r="B21" s="34" t="s">
         <v>483</v>
       </c>
-      <c r="C21" s="47" t="s">
-        <v>541</v>
-      </c>
-      <c r="D21" s="47" t="s">
-        <v>541</v>
+      <c r="C21" s="46" t="s">
+        <v>532</v>
+      </c>
+      <c r="D21" s="46" t="s">
+        <v>532</v>
       </c>
       <c r="E21" s="32" t="s">
         <v>486</v>
       </c>
       <c r="F21" s="32" t="s">
-        <v>542</v>
+        <v>533</v>
       </c>
       <c r="G21" s="32" t="s">
         <v>488</v>
       </c>
       <c r="H21" s="33" t="s">
-        <v>543</v>
+        <v>534</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="150" x14ac:dyDescent="0.2">
       <c r="A22" s="26" t="s">
-        <v>544</v>
+        <v>535</v>
       </c>
       <c r="B22" s="34" t="s">
         <v>483</v>
       </c>
-      <c r="C22" s="47" t="s">
-        <v>545</v>
-      </c>
-      <c r="D22" s="47" t="s">
-        <v>545</v>
+      <c r="C22" s="46" t="s">
+        <v>536</v>
+      </c>
+      <c r="D22" s="46" t="s">
+        <v>536</v>
       </c>
       <c r="E22" s="32" t="s">
         <v>486</v>
       </c>
       <c r="F22" s="32" t="s">
-        <v>542</v>
+        <v>533</v>
       </c>
       <c r="G22" s="32" t="s">
         <v>488</v>
       </c>
       <c r="H22" s="33" t="s">
-        <v>546</v>
+        <v>537</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations disablePrompts="1" count="2">
+  <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E6:E22">
       <formula1>"Critical,Serious, Minor, Tweak"</formula1>
     </dataValidation>

</xml_diff>